<commit_message>
Agrega estimación de gastos y estilo de pagina tesoreria
</commit_message>
<xml_diff>
--- a/data/miembros.xlsx
+++ b/data/miembros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Desktop/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{C40AC0FF-3A7F-4E5D-AB99-CBECBAF74402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C34164DC-3819-BF4E-92BA-C551442F3677}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="13_ncr:1_{C40AC0FF-3A7F-4E5D-AB99-CBECBAF74402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50076FF2-DC7A-7E4B-A2AC-B242BAF43AC2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26000" windowHeight="16000" xr2:uid="{E69FF370-BCB9-4155-8F01-725C61F4E151}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26980" windowHeight="16340" activeTab="1" xr2:uid="{E69FF370-BCB9-4155-8F01-725C61F4E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de miembros" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="104">
   <si>
     <t>Franddy</t>
   </si>
@@ -214,9 +214,6 @@
     <t>Amparo</t>
   </si>
   <si>
-    <t xml:space="preserve">Kibel </t>
-  </si>
-  <si>
     <t>Payano</t>
   </si>
   <si>
@@ -329,6 +326,18 @@
   </si>
   <si>
     <t>apodo</t>
+  </si>
+  <si>
+    <t>estatus</t>
+  </si>
+  <si>
+    <t>Santo</t>
+  </si>
+  <si>
+    <t>Inactivo</t>
+  </si>
+  <si>
+    <t>Activo</t>
   </si>
 </sst>
 </file>
@@ -383,12 +392,18 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -403,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -415,30 +430,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE220CC2-8725-42B3-AD79-7FD328EB1B49}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1126,16 +1150,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C9BEE0-E0C8-294A-8E6C-D5BDC9887771}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:F14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="12"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
@@ -1143,544 +1171,650 @@
         <v>26</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10">
+      <c r="D2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="2">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F2" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F3" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F4" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10">
+      <c r="D5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F5" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F6" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="11">
+      <c r="E7" s="9">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F7" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="10">
+      <c r="C8" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F8" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10">
+      <c r="C9" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F9" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F10" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="10">
+      <c r="E11" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F11" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10">
+      <c r="C12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F12" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="2">
+        <v>21</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="13">
+        <v>13</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
-        <v>13</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10">
+      <c r="D14" s="15"/>
+      <c r="E14" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F14" s="17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10">
+      <c r="C15" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F15" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10">
+      <c r="C16" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F16" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="10">
+      <c r="E17" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F17" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10">
+      <c r="C18" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F18" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10">
+      <c r="C19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F19" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10">
+      <c r="C20" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F20" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10">
+      <c r="C21" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F21" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="10">
+      <c r="D22" s="8"/>
+      <c r="E22" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F22" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="10">
+      <c r="C23" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F23" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>23</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="10">
+      <c r="C24" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F24" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>24</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="10">
+      <c r="C25" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="2">
         <v>92</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F25" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="10">
+      <c r="B26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F26" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>26</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="10">
+      <c r="C27" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="2">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F27" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="13">
+      <c r="C28" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="4">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F28" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>28</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="13">
+      <c r="C29" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="4">
         <v>22</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>29</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="13">
+      <c r="E30" s="4">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F30" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>30</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="9"/>
-      <c r="E31" s="13">
+      <c r="C31" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F31" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>31</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="13">
+      <c r="C32" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="4">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F32" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>32</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D33" s="9"/>
-      <c r="E33" s="13">
+      <c r="C33" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>33</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="13">
+      <c r="E34" s="4">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>34</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="13">
+      <c r="E35" s="4">
         <v>27</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="F35" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>35</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="13">
+      <c r="C36" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" s="8"/>
+      <c r="E36" s="4">
         <v>45</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aportes table wider width
</commit_message>
<xml_diff>
--- a/data/miembros.xlsx
+++ b/data/miembros.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26306"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Desktop/proyectos_r/1-personales/goat/website/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Backup/proyectos_r/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="13_ncr:1_{C40AC0FF-3A7F-4E5D-AB99-CBECBAF74402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50076FF2-DC7A-7E4B-A2AC-B242BAF43AC2}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="13_ncr:1_{C40AC0FF-3A7F-4E5D-AB99-CBECBAF74402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CEA8598-7760-3446-85AC-3A9C7356C46A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26980" windowHeight="16340" firstSheet="1" activeTab="1" xr2:uid="{E69FF370-BCB9-4155-8F01-725C61F4E151}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26980" windowHeight="16340" activeTab="1" xr2:uid="{E69FF370-BCB9-4155-8F01-725C61F4E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de miembros" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="miembros" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="105">
   <si>
     <t>id</t>
   </si>
@@ -333,9 +333,6 @@
     <t>Pimentel</t>
   </si>
   <si>
-    <t>Amio de Kibelo</t>
-  </si>
-  <si>
     <t>Bello</t>
   </si>
   <si>
@@ -349,13 +346,19 @@
   </si>
   <si>
     <t>Valdez</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -790,17 +793,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE220CC2-8725-42B3-AD79-7FD328EB1B49}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -814,7 +817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -825,7 +828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -836,7 +839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -847,7 +850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -858,7 +861,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -872,7 +875,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -886,7 +889,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -894,7 +897,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -905,7 +908,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -916,7 +919,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -927,7 +930,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -935,7 +938,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -949,7 +952,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -957,7 +960,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -968,7 +971,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -976,7 +979,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -987,7 +990,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -995,7 +998,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1003,7 +1006,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1011,7 +1014,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1022,7 +1025,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1038,7 +1041,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -1046,7 +1049,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -1054,7 +1057,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -1062,7 +1065,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -1073,7 +1076,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -1092,7 +1095,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -1103,7 +1106,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -1111,7 +1114,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -1122,7 +1125,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -1130,7 +1133,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -1141,7 +1144,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -1157,20 +1160,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C9BEE0-E0C8-294A-8E6C-D5BDC9887771}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:F14"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="12"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="12"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1189,8 +1192,11 @@
       <c r="F1" s="11" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.95">
+      <c r="G1" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1210,7 +1216,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.95">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1230,7 +1236,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.95">
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -1250,7 +1256,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.95">
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -1270,7 +1276,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.95">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1290,7 +1296,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.95">
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1310,7 +1316,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.95">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -1328,7 +1334,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.95">
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -1346,7 +1352,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.95">
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -1364,7 +1370,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.95">
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1384,7 +1390,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.95">
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -1402,7 +1408,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.95">
+    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -1420,7 +1426,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.95">
+    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
         <v>13</v>
       </c>
@@ -1438,7 +1444,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.95">
+    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -1456,7 +1462,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.95">
+    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -1474,7 +1480,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.95">
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -1494,7 +1500,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.95">
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -1512,7 +1518,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.95">
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>18</v>
       </c>
@@ -1530,7 +1536,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.95">
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -1548,7 +1554,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.95">
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -1566,7 +1572,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.95">
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -1584,7 +1590,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.95">
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -1602,7 +1608,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.95">
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>23</v>
       </c>
@@ -1620,7 +1626,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.95">
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>24</v>
       </c>
@@ -1638,12 +1644,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.95">
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>87</v>
@@ -1656,7 +1662,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.95">
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -1664,7 +1670,7 @@
         <v>43</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="2">
@@ -1674,7 +1680,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.95">
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="7">
         <v>27</v>
       </c>
@@ -1682,7 +1688,7 @@
         <v>44</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="4">
@@ -1692,7 +1698,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.95">
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>28</v>
       </c>
@@ -1700,7 +1706,7 @@
         <v>46</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="4">
@@ -1710,7 +1716,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="7">
         <v>29</v>
       </c>
@@ -1724,7 +1730,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.95">
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>30</v>
       </c>
@@ -1742,7 +1748,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.95">
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="7">
         <v>31</v>
       </c>
@@ -1760,7 +1766,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.95">
+    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>32</v>
       </c>
@@ -1768,7 +1774,7 @@
         <v>52</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="4">
@@ -1778,7 +1784,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>33</v>
       </c>
@@ -1792,7 +1798,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>34</v>
       </c>
@@ -1806,7 +1812,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.95">
+    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="7">
         <v>35</v>
       </c>
@@ -1814,7 +1820,7 @@
         <v>57</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="4">
@@ -1822,6 +1828,9 @@
       </c>
       <c r="F36" s="12" t="s">
         <v>85</v>
+      </c>
+      <c r="G36" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Conditional style based on payment
</commit_message>
<xml_diff>
--- a/data/miembros.xlsx
+++ b/data/miembros.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/Backup/proyectos_r/1-personales/goat/website/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8feae05406065f8f/[5] R projects/1-personales/goat/website/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="13_ncr:1_{C40AC0FF-3A7F-4E5D-AB99-CBECBAF74402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{499766CD-2D53-BA42-A2DC-6EAF79E169A2}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{C40AC0FF-3A7F-4E5D-AB99-CBECBAF74402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36CBE432-72C1-DE42-82C1-130D53970CE2}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{E69FF370-BCB9-4155-8F01-725C61F4E151}"/>
   </bookViews>
@@ -785,8 +785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C9BEE0-E0C8-294A-8E6C-D5BDC9887771}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -862,7 +862,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>34</v>

</xml_diff>